<commit_message>
Extra BETA 0.3.1 支持
</commit_message>
<xml_diff>
--- a/内部编号列表/[hack]Ultra Wide Expansion.xlsx
+++ b/内部编号列表/[hack]Ultra Wide Expansion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7860"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="20240806 单人玩家" sheetId="1" r:id="rId1"/>
@@ -5701,8 +5701,8 @@
   <sheetPr/>
   <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="F34" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20" customHeight="1"/>
@@ -5710,15 +5710,15 @@
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="14.25" style="2" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="14.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.8796296296296" style="1" customWidth="1"/>
     <col min="7" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="14.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5555555555556" style="1" customWidth="1"/>
     <col min="10" max="12" width="9" style="1"/>
     <col min="13" max="13" width="30" style="3" customWidth="1"/>
     <col min="14" max="15" width="9" style="1"/>
-    <col min="16" max="16" width="18.625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6296296296296" style="1" customWidth="1"/>
     <col min="17" max="18" width="9" style="1"/>
-    <col min="19" max="19" width="29.875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="29.8796296296296" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>

</xml_diff>